<commit_message>
Updated pins to be correct
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\workspace\YSU-Micromouse-SAC-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Tyler\workspace\YSU-Micromouse-SAC-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Pins</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Teensy</t>
   </si>
@@ -69,14 +66,79 @@
   </si>
   <si>
     <t>A15</t>
+  </si>
+  <si>
+    <t>Analog Name</t>
+  </si>
+  <si>
+    <t>In/Out</t>
+  </si>
+  <si>
+    <t>Analog/Digital</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>L Encoder A</t>
+  </si>
+  <si>
+    <t>L Encoder B</t>
+  </si>
+  <si>
+    <t>R Encoder A</t>
+  </si>
+  <si>
+    <t>R Encoder B</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Analog</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>AIN2</t>
+  </si>
+  <si>
+    <t>AIN1</t>
+  </si>
+  <si>
+    <t>PWMA</t>
+  </si>
+  <si>
+    <t>PWMB</t>
+  </si>
+  <si>
+    <t>BIN1</t>
+  </si>
+  <si>
+    <t>BIN2</t>
+  </si>
+  <si>
+    <t>Motor Driver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,115 +483,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated pins to new configuration
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Pins</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>A15</t>
+  </si>
+  <si>
+    <t>Left Encoder A</t>
+  </si>
+  <si>
+    <t>Left Encoder B</t>
+  </si>
+  <si>
+    <t>Right Encoder A</t>
+  </si>
+  <si>
+    <t>Right Encoder B</t>
   </si>
 </sst>
 </file>
@@ -420,15 +432,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -441,10 +454,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,39 +465,39 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,39 +505,71 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B15">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>